<commit_message>
New files: UML/Проект Расписание  Вариант 8.pptx UML/Scheduler_classes_14.puml
</commit_message>
<xml_diff>
--- a/input/Расписание №13 Form.xlsx
+++ b/input/Расписание №13 Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mission\5.Programming\pythonProject\University-Schedule-Planner\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AEC7CB-BC60-4514-A620-43F053D0C545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A3D839-8839-421E-9C12-B5001494F553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32640" yWindow="6360" windowWidth="20892" windowHeight="13188" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -521,7 +521,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,7 +593,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>13</v>
@@ -619,7 +619,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>11</v>
@@ -671,7 +671,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>18</v>
@@ -703,7 +703,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>18</v>
@@ -735,7 +735,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>18</v>

</xml_diff>